<commit_message>
feature: topluluk ekibimiz page initialized
</commit_message>
<xml_diff>
--- a/input/Topluluk Ekibi.xlsx
+++ b/input/Topluluk Ekibi.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>İsim</t>
   </si>
@@ -22,16 +22,25 @@
     <t>Rol</t>
   </si>
   <si>
+    <t>Linkedin</t>
+  </si>
+  <si>
     <t>Oğuz Ergin</t>
   </si>
   <si>
     <t>Kurucu ve Danışman Hoca</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/oguzergin</t>
+  </si>
+  <si>
     <t>Ata Turhan</t>
   </si>
   <si>
     <t>Kurucu ve Topluluk Başkanı</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ata-turhan-555b5b160/</t>
   </si>
   <si>
     <t>Recep Çankaya</t>
@@ -63,12 +72,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +86,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -84,36 +108,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -121,7 +118,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -129,39 +126,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -199,14 +164,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -214,6 +171,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -223,6 +196,35 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,25 +239,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,157 +413,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,30 +430,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -466,17 +444,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,6 +473,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -523,161 +514,173 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,75 +1000,87 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="14.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="20.7777777777778" customWidth="1"/>
+    <col min="2" max="2" width="34.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="https://www.linkedin.com/in/oguzergin"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
feature: etkinlik takvimi page initialized
</commit_message>
<xml_diff>
--- a/input/Topluluk Ekibi.xlsx
+++ b/input/Topluluk Ekibi.xlsx
@@ -40,7 +40,7 @@
     <t>Kurucu ve Topluluk Başkanı</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/ata-turhan-555b5b160/</t>
+    <t>https://www.linkedin.com/in/ata-turhan/</t>
   </si>
   <si>
     <t>Recep Çankaya</t>
@@ -72,10 +72,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -108,25 +108,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,6 +163,21 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -171,16 +201,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -188,43 +224,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,187 +239,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,6 +430,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -489,9 +498,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -510,176 +530,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1003,7 +1004,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -1041,7 +1042,7 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1080,6 +1081,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://www.linkedin.com/in/oguzergin"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://www.linkedin.com/in/ata-turhan/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feature: linkedin profiles added to ekip page
</commit_message>
<xml_diff>
--- a/input/Topluluk Ekibi.xlsx
+++ b/input/Topluluk Ekibi.xlsx
@@ -43,7 +43,7 @@
     <t>https://www.linkedin.com/in/ata-turhan/</t>
   </si>
   <si>
-    <t>Recep Çankaya</t>
+    <t>Beyazıt Nural</t>
   </si>
   <si>
     <t>Blockchain Kulübü Başkanı</t>
@@ -72,9 +72,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -95,37 +95,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,21 +148,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -201,6 +171,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -208,6 +194,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -215,7 +209,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -225,6 +218,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,187 +239,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,24 +435,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,20 +485,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -530,158 +506,182 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
feature: new page added
</commit_message>
<xml_diff>
--- a/input/Topluluk Ekibi.xlsx
+++ b/input/Topluluk Ekibi.xlsx
@@ -189,10 +189,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -218,6 +218,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -225,32 +233,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,6 +280,29 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -280,68 +310,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -362,6 +362,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -374,61 +404,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,103 +536,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,11 +550,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -598,28 +615,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -650,15 +650,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -668,127 +668,127 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1120,7 +1120,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
design and refactor: team page redesigned and os path used for os compatibility
</commit_message>
<xml_diff>
--- a/input/Topluluk Ekibi.xlsx
+++ b/input/Topluluk Ekibi.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>İsim</t>
   </si>
@@ -83,12 +83,6 @@
   </si>
   <si>
     <t>çağrı-çiftgül-710bb1197</t>
-  </si>
-  <si>
-    <t>Doğukan Yıldırım</t>
-  </si>
-  <si>
-    <t>doğukan-yıldırım-790212230</t>
   </si>
   <si>
     <t>Deniz Yıldırım</t>
@@ -189,9 +183,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
@@ -212,12 +206,34 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -226,6 +242,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -234,30 +251,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,13 +288,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -312,9 +306,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -326,7 +320,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -341,7 +335,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,181 +350,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,6 +541,35 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -561,17 +584,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -615,15 +627,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -638,27 +641,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -668,130 +662,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1117,10 +1111,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1233,24 +1227,24 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
@@ -1261,7 +1255,7 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -1275,7 +1269,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -1289,38 +1283,38 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
         <v>39</v>
@@ -1331,24 +1325,24 @@
         <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
         <v>44</v>
@@ -1359,7 +1353,7 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
@@ -1373,7 +1367,7 @@
         <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
@@ -1387,41 +1381,27 @@
         <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>